<commit_message>
Nathan's hours wk 4
</commit_message>
<xml_diff>
--- a/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
+++ b/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23206294_student_uwa_edu_au/Documents/CITS3200/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23206294_student_uwa_edu_au/Documents/CITS3200/italian_3200_project/documentation/booked_hours_individual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{650621C6-2C58-45A3-AC14-70BE0756C40F}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E983F1F-917D-7946-91D1-62D5F68452E3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Wk</t>
   </si>
@@ -75,12 +75,6 @@
     <t>First online meeting with group members</t>
   </si>
   <si>
-    <t>Formal meeting</t>
-  </si>
-  <si>
-    <t>Preparing skills and resources audit deliverable</t>
-  </si>
-  <si>
     <t>Researching audio similarity software/libraries &amp; implementation of scoring metrics</t>
   </si>
   <si>
@@ -94,17 +88,36 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Lucida Sans"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
     </r>
+  </si>
+  <si>
+    <t>Created skills audit survey</t>
+  </si>
+  <si>
+    <t>Formal team meeting</t>
+  </si>
+  <si>
+    <t>Distributed skills audit survey to group members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formatted skills audit deliverable </t>
+  </si>
+  <si>
+    <t>Preperation for skills and resources audit deliverable</t>
+  </si>
+  <si>
+    <t>Set up basic flask project template</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -113,19 +126,23 @@
       <b/>
       <sz val="12"/>
       <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Lucida Sans Typewriter"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -293,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -316,6 +333,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -365,27 +391,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,6 +475,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -796,60 +805,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="3.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.75" style="1"/>
-    <col min="9" max="9" width="10.75" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.75" style="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="1:9" ht="71" customHeight="1">
+      <c r="A1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:9" ht="13" customHeight="1">
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -862,24 +871,24 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3" s="21"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="4">
         <v>43671</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="4">
         <v>43671</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="5">
         <v>0.45833333333333331</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -898,52 +907,52 @@
         <v>1.0000000001164153</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="4">
         <v>43679</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="5">
         <v>0.375</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="4">
         <v>43679</v>
       </c>
-      <c r="E5" s="21">
-        <v>0.39583333333333331</v>
+      <c r="E5" s="5">
+        <v>0.3888888888888889</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="6">
         <f>IF(I5&gt;0,I5,IF(I5=0, " ", "ERROR"))</f>
-        <v>0.50000000005820766</v>
+        <v>0.33333333337213844</v>
       </c>
       <c r="H5" s="1">
         <f>IF(AND(G5&lt;&gt;" ",G5&lt;&gt;"ERROR",H4&lt;&gt;" ", H4&lt;&gt;"ERROR"),G5+H4," ")</f>
-        <v>1.500000000174623</v>
+        <v>1.3333333334885538</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I68" si="0">((D5+E5)-(B5+C5))*24</f>
-        <v>0.50000000005820766</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.33333333337213844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="4">
         <v>43679</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="5">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="4">
         <v>43679</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -955,27 +964,27 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6:H30" si="2">IF(AND(G6&lt;&gt;" ",G6&lt;&gt;"ERROR",H5&lt;&gt;" ", H5&lt;&gt;"ERROR"),G6+H5," ")</f>
-        <v>2.0000000000582077</v>
+        <v>1.8333333333721384</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>0.49999999988358468</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="4">
         <v>43681</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="5">
         <v>0.75</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="4">
         <v>43681</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="5">
         <v>0.79166666666666663</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -987,31 +996,31 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2.8333333333139308</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>0.99999999994179234</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="4">
         <v>43683</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="7">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="8">
         <v>43683</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="7">
         <v>0.4513888888888889</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
+      <c r="F8" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="1"/>
@@ -1019,31 +1028,31 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>4.3333333333139308</v>
+        <v>4.1666666666278616</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>1.3333333333139308</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="8">
         <v>43685</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="5">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="8">
         <v>43685</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="5">
         <v>0.77083333333333337</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="1"/>
@@ -1051,31 +1060,31 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="2"/>
-        <v>5.8333333333139308</v>
+        <v>5.6666666666278616</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="4">
         <v>43656</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="4">
         <v>43656</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="1"/>
@@ -1083,136 +1092,206 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5.8333333333139308</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0.16666666668606922</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="4">
         <v>43656</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="4">
         <v>43656</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="22">
+      <c r="F11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6">
         <f t="shared" ref="G11" si="3">IF(I11&gt;0,I11,IF(I11=0, " ", "ERROR"))</f>
         <v>1.5</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="1">
         <f t="shared" ref="H11" si="4">IF(AND(G11&lt;&gt;" ",G11&lt;&gt;"ERROR",H10&lt;&gt;" ", H10&lt;&gt;"ERROR"),G11+H10," ")</f>
-        <v>7.5</v>
+        <v>7.3333333333139308</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="G12" s="6" t="str">
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>43689</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="4">
+        <v>43689</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H12" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>8.3333333332557231</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="G13" s="6" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="4">
+        <v>43690</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D13" s="4">
+        <v>43690</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H13" s="1" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>9.8333333332557231</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="G14" s="6" t="str">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <v>43690</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43690</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H14" s="1" t="str">
+        <v>0.16666666668606922</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>9.9999999999417923</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="G15" s="6" t="str">
+        <v>0.16666666668606922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43691</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D15" s="4">
+        <v>43691</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H15" s="1" t="str">
+        <v>1.0000000001164153</v>
+      </c>
+      <c r="H15" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>11.000000000058208</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="G16" s="6" t="str">
+        <v>1.0000000001164153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4">
+        <v>43694</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="D16" s="4">
+        <v>43694</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H16" s="1" t="str">
+        <v>0.33333333337213844</v>
+      </c>
+      <c r="H16" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>11.333333333430346</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.33333333337213844</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
@@ -1230,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
@@ -1248,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
@@ -1266,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
@@ -1284,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
@@ -1302,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
@@ -1320,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="4"/>
@@ -1338,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="4"/>
@@ -1356,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
@@ -1374,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
@@ -1392,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
@@ -1410,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="4"/>
@@ -1428,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
@@ -1446,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="4"/>
@@ -1464,25 +1543,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="15" t="s">
+    <row r="31" spans="1:9" ht="16">
+      <c r="A31" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="7" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I31" s="1" t="e">
@@ -1490,8 +1569,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+    <row r="32" spans="1:9" ht="16">
+      <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1504,15 +1583,15 @@
       <c r="E32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
@@ -1530,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9">
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="4"/>
@@ -1548,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9">
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="4"/>
@@ -1566,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9">
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="4"/>
@@ -1584,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9">
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
@@ -1602,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9">
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="4"/>
@@ -1620,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9">
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="4"/>
@@ -1638,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9">
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="4"/>
@@ -1656,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9">
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
@@ -1674,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9">
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
@@ -1692,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9">
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
@@ -1710,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9">
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
@@ -1728,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9">
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
@@ -1746,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9">
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="4"/>
@@ -1764,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9">
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="4"/>
@@ -1782,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9">
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="4"/>
@@ -1800,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9">
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="4"/>
@@ -1818,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9">
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="4"/>
@@ -1836,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9">
       <c r="B51" s="4"/>
       <c r="C51" s="5"/>
       <c r="D51" s="4"/>
@@ -1854,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9">
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="4"/>
@@ -1872,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9">
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
       <c r="D53" s="4"/>
@@ -1890,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9">
       <c r="B54" s="4"/>
       <c r="C54" s="5"/>
       <c r="D54" s="4"/>
@@ -1908,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9">
       <c r="B55" s="4"/>
       <c r="C55" s="5"/>
       <c r="D55" s="4"/>
@@ -1926,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9">
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
       <c r="D56" s="4"/>
@@ -1944,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9">
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
       <c r="D57" s="4"/>
@@ -1962,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9">
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
       <c r="D58" s="4"/>
@@ -1980,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9">
       <c r="B59" s="4"/>
       <c r="C59" s="5"/>
       <c r="D59" s="4"/>
@@ -1998,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9">
       <c r="B60" s="4"/>
       <c r="G60" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2013,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9">
       <c r="B61" s="4"/>
       <c r="G61" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2028,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9">
       <c r="B62" s="4"/>
       <c r="G62" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2043,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9">
       <c r="B63" s="4"/>
       <c r="G63" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2058,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9">
       <c r="B64" s="4"/>
       <c r="G64" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2073,25 +2152,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="15" t="s">
+    <row r="65" spans="1:9" ht="16">
+      <c r="A65" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="15" t="s">
+      <c r="C65" s="19"/>
+      <c r="D65" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="16"/>
-      <c r="F65" s="7" t="s">
+      <c r="E65" s="19"/>
+      <c r="F65" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="G65" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="H65" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I65" s="1" t="e">
@@ -2099,8 +2178,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="9"/>
+    <row r="66" spans="1:9" ht="16">
+      <c r="A66" s="12"/>
       <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
@@ -2113,15 +2192,15 @@
       <c r="E66" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
       <c r="I66" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9">
       <c r="G67" s="6" t="str">
         <f t="shared" ref="G67:G98" si="7">IF(I67&gt;0,I67,IF(I67=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
@@ -2135,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9">
       <c r="G68" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2149,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9">
       <c r="G69" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2163,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9">
       <c r="G70" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2177,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9">
       <c r="G71" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2191,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9">
       <c r="G72" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2205,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9">
       <c r="G73" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2219,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9">
       <c r="G74" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2233,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9">
       <c r="G75" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2247,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="G76" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2261,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9">
       <c r="G77" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2275,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9">
       <c r="G78" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2289,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9">
       <c r="G79" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2303,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9">
       <c r="G80" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2317,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="7:9">
       <c r="G81" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2331,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="7:9">
       <c r="G82" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2345,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="7:9">
       <c r="G83" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2359,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="7:9">
       <c r="G84" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2373,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="7:9">
       <c r="G85" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2387,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="7:9">
       <c r="G86" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2401,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="7:9">
       <c r="G87" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2415,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="7:9">
       <c r="G88" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2429,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="7:9">
       <c r="G89" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2443,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="7:9">
       <c r="G90" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2457,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="7:9">
       <c r="G91" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2471,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="7:9">
       <c r="G92" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2485,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="7:9">
       <c r="G93" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2499,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="7:9">
       <c r="G94" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2513,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="7:9">
       <c r="G95" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2527,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="7:9">
       <c r="G96" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2541,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9">
       <c r="G97" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2555,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9">
       <c r="G98" s="6" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -2569,25 +2648,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B99" s="15" t="s">
+    <row r="99" spans="1:9" ht="16">
+      <c r="A99" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="16"/>
-      <c r="D99" s="15" t="s">
+      <c r="C99" s="19"/>
+      <c r="D99" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E99" s="16"/>
-      <c r="F99" s="7" t="s">
+      <c r="E99" s="19"/>
+      <c r="F99" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G99" s="7" t="s">
+      <c r="G99" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H99" s="7" t="s">
+      <c r="H99" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I99" s="1" t="e">
@@ -2595,8 +2674,8 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="9"/>
+    <row r="100" spans="1:9" ht="16">
+      <c r="A100" s="12"/>
       <c r="B100" s="2" t="s">
         <v>2</v>
       </c>
@@ -2609,15 +2688,15 @@
       <c r="E100" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="7"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
       <c r="I100" s="1" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9">
       <c r="G101" s="6" t="str">
         <f t="shared" ref="G101:G132" si="10">IF(I101&gt;0,I101,IF(I101=0, " ", "ERROR"))</f>
         <v xml:space="preserve"> </v>
@@ -2631,7 +2710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9">
       <c r="G102" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2645,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9">
       <c r="G103" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2659,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9">
       <c r="G104" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2673,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9">
       <c r="G105" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2687,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9">
       <c r="G106" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2701,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9">
       <c r="G107" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2715,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9">
       <c r="G108" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2729,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9">
       <c r="G109" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2743,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9">
       <c r="G110" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2757,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9">
       <c r="G111" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2771,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9">
       <c r="G112" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2785,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="7:9">
       <c r="G113" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2799,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="7:9">
       <c r="G114" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2813,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="7:9">
       <c r="G115" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2827,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="7:9">
       <c r="G116" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2841,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="7:9">
       <c r="G117" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2855,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="7:9">
       <c r="G118" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2869,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="7:9">
       <c r="G119" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2883,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="7:9">
       <c r="G120" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2897,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="7:9">
       <c r="G121" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2911,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="7:9">
       <c r="G122" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2925,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="7:9">
       <c r="G123" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2939,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="7:9">
       <c r="G124" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2953,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="7:9">
       <c r="G125" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2967,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="7:9">
       <c r="G126" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2981,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="7:9">
       <c r="G127" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -2995,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="7:9">
       <c r="G128" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -3009,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="7:9">
       <c r="G129" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -3023,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="7:9">
       <c r="G130" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -3037,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="7:9">
       <c r="G131" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -3051,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="7:9">
       <c r="G132" s="6" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
@@ -3106,7 +3185,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="256" width="11" customWidth="1"/>
   </cols>
@@ -3124,7 +3203,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="256" width="11" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Nathan's hours wk 5
</commit_message>
<xml_diff>
--- a/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
+++ b/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23206294_student_uwa_edu_au/Documents/CITS3200/italian_3200_project/documentation/booked_hours_individual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E983F1F-917D-7946-91D1-62D5F68452E3}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:40009_{3CF58E6A-5DF7-4373-BB5C-FF4A4CCF2CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2201DE2C-68F0-664F-AF14-E6FA28DBBBAA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>Wk</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Set up basic flask project template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on backend </t>
+  </si>
+  <si>
+    <t>Researching database integration</t>
   </si>
 </sst>
 </file>
@@ -356,6 +362,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -374,14 +388,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -475,10 +481,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -805,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
@@ -824,36 +826,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="71" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -873,7 +875,7 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="17"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
@@ -1292,57 +1294,99 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="G17" s="6" t="str">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>43697</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D17" s="4">
+        <v>43697</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H17" s="1" t="str">
+        <v>0.6666666665696539</v>
+      </c>
+      <c r="H17" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>12</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6666666665696539</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-      <c r="G18" s="6" t="str">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4">
+        <v>43699</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43699</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H18" s="1" t="str">
+        <v>2.0000000000582077</v>
+      </c>
+      <c r="H18" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>14.000000000058208</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0000000000582077</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="G19" s="6" t="str">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43700</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D19" s="4">
+        <v>43700</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H19" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H19" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>15</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1547,14 +1591,14 @@
       <c r="A31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="18" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="19"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="10" t="s">
         <v>5</v>
       </c>
@@ -2156,14 +2200,14 @@
       <c r="A65" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="18" t="s">
+      <c r="C65" s="14"/>
+      <c r="D65" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="19"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,14 +2696,14 @@
       <c r="A99" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="19"/>
-      <c r="D99" s="18" t="s">
+      <c r="C99" s="14"/>
+      <c r="D99" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E99" s="19"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="10" t="s">
         <v>5</v>
       </c>
@@ -3146,18 +3190,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H99:H100"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:F100"/>
-    <mergeCell ref="G99:G100"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:F66"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A1:H1"/>
@@ -3171,6 +3203,18 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="H99:H100"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="G99:G100"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Nathan's hours wk 7
</commit_message>
<xml_diff>
--- a/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
+++ b/documentation/booked_hours_individual/Booked_Hours_NathanONeill.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanoneill/OneDrive - The University of Western Australia/CITS3200/italian_3200_project/documentation/booked_hours_individual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/23206294_student_uwa_edu_au/Documents/CITS3200/italian_3200_project/documentation/booked_hours_individual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15495690-BE78-784B-9B84-F93B2EA67AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{15495690-BE78-784B-9B84-F93B2EA67AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E35967DE-5375-6D43-A384-263AFC3E0DF1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Wk</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t xml:space="preserve">Began registration form </t>
+  </si>
+  <si>
+    <t>Team meeting (study break)</t>
+  </si>
+  <si>
+    <t>Set up Auth0 app &amp; integrated API</t>
+  </si>
+  <si>
+    <t>Set up basic login button template, created routing for profile access</t>
+  </si>
+  <si>
+    <t>Client briefing/meeting</t>
+  </si>
+  <si>
+    <t>Testing Auth0 authorisation methods</t>
   </si>
 </sst>
 </file>
@@ -368,6 +383,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -386,14 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -813,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="137" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
@@ -832,36 +847,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="71" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -881,7 +896,7 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="17"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
@@ -1492,114 +1507,201 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="G23" s="6" t="str">
+      <c r="A23" s="1">
+        <v>7</v>
+      </c>
+      <c r="B23" s="4">
+        <v>43711</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D23" s="4">
+        <v>43711</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H23" s="1" t="str">
+        <v>0.49999999988358468</v>
+      </c>
+      <c r="H23" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>18.8333333330811</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.49999999988358468</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="G24" s="6" t="str">
+      <c r="A24" s="1">
+        <v>7</v>
+      </c>
+      <c r="B24" s="4">
+        <v>43714</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43714</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H24" s="1" t="str">
+        <v>3.9999999999417923</v>
+      </c>
+      <c r="H24" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>22.833333333022892</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.9999999999417923</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="G25" s="6" t="str">
+      <c r="A25" s="1">
+        <v>7</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43715</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D25" s="4">
+        <v>43715</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H25" s="1" t="str">
+        <v>0.99999999994179234</v>
+      </c>
+      <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>23.833333332964685</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99999999994179234</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="G26" s="6" t="str">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" s="4">
+        <v>43718</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="D26" s="4">
+        <v>43718</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H26" s="1" t="str">
+        <v>0.50000000005820766</v>
+      </c>
+      <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>24.333333333022892</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.50000000005820766</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="G27" s="6" t="str">
+      <c r="A27" s="1">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4">
+        <v>43718</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D27" s="4">
+        <v>43718</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H27" s="1" t="str">
+        <v>0.50000000005820766</v>
+      </c>
+      <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>24.8333333330811</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.50000000005820766</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="G28" s="6" t="str">
+      <c r="A28" s="1">
+        <v>7</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43722</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D28" s="4">
+        <v>43722</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="6">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H28" s="1" t="str">
+        <v>1.9999999998835847</v>
+      </c>
+      <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v xml:space="preserve"> </v>
+        <v>26.833333332964685</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9999999998835847</v>
       </c>
     </row>
     <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>7</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
@@ -1639,14 +1741,14 @@
       <c r="A31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="18" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="19"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="10" t="s">
         <v>5</v>
       </c>
@@ -2248,14 +2350,14 @@
       <c r="A65" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="18" t="s">
+      <c r="C65" s="14"/>
+      <c r="D65" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="19"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="10" t="s">
         <v>5</v>
       </c>
@@ -2744,14 +2846,14 @@
       <c r="A99" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="19"/>
-      <c r="D99" s="18" t="s">
+      <c r="C99" s="14"/>
+      <c r="D99" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E99" s="19"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="10" t="s">
         <v>5</v>
       </c>
@@ -3238,18 +3340,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H99:H100"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:F100"/>
-    <mergeCell ref="G99:G100"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:F66"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A1:H1"/>
@@ -3263,6 +3353,18 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="H99:H100"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="G99:G100"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>